<commit_message>
Added fun magent and description fix
</commit_message>
<xml_diff>
--- a/fun_test/web/static/logs/hu_performance.xlsx
+++ b/fun_test/web/static/logs/hu_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ash/Desktop/Integration/fun_test/web/static/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988359C9-27D3-A044-8BD0-8D38E0DC4E2D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFDAFD9-F78E-4643-9DA4-A6B88D114B45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37560" yWindow="2600" windowWidth="46660" windowHeight="23820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>RAW VOLUME/NS</t>
   </si>
@@ -197,10 +197,22 @@
     <t>IO per second</t>
   </si>
   <si>
-    <t>threads</t>
+    <t>Testbed</t>
   </si>
   <si>
-    <t>Number of threads</t>
+    <t>storage2</t>
+  </si>
+  <si>
+    <t>storage1</t>
+  </si>
+  <si>
+    <t>storagenw</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>testbed</t>
   </si>
 </sst>
 </file>
@@ -326,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -342,6 +354,7 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -350,7 +363,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +715,10 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -726,11 +739,11 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -750,10 +763,10 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -766,11 +779,11 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4" t="s">
@@ -1082,11 +1095,11 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1109,11 +1122,11 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="4" t="s">
@@ -11961,32 +11974,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F373BE-429C-1740-BE96-AE8CB8CA1AC8}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="44.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="8"/>
-    <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="8"/>
-    <col min="9" max="9" width="12.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="3" width="44.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="8"/>
+    <col min="8" max="8" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="8"/>
+    <col min="10" max="10" width="12.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="8" t="s">
@@ -12060,84 +12074,121 @@
     </row>
     <row r="7" spans="1:12" ht="16">
       <c r="A7" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" ht="16">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="16">
+      <c r="A10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="16">
+      <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18">
+      <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="16">
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" ht="16">
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" ht="16">
-      <c r="A11" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="16">
-      <c r="A13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="8">
+        <v>31</v>
+      </c>
+      <c r="C15" s="10">
+        <v>183</v>
+      </c>
+      <c r="D15" s="11">
+        <v>124</v>
+      </c>
+      <c r="E15" s="15">
+        <f ca="1">NOW()</f>
+        <v>43320.529748726854</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" ht="18">
+      <c r="A16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="8">
         <v>57</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="18">
-      <c r="A16" s="8">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8">
-        <v>31</v>
-      </c>
       <c r="C16" s="10">
-        <v>183</v>
-      </c>
-      <c r="D16" s="11">
-        <v>124</v>
-      </c>
-      <c r="E16" s="21">
+        <v>101</v>
+      </c>
+      <c r="D16" s="10">
+        <v>228</v>
+      </c>
+      <c r="E16" s="22">
         <f ca="1">NOW()</f>
-        <v>43315.588381250003</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+        <v>43320.529748726854</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="18">
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+    <row r="17" spans="1:14" ht="18">
+      <c r="A17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3.161</v>
+      </c>
+      <c r="C17" s="10">
+        <v>15172.23</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3.1579999999999999</v>
+      </c>
+      <c r="E17" s="22">
+        <f ca="1">NOW()</f>
+        <v>43320.529748726854</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -12146,8 +12197,7 @@
       <c r="K17" s="10"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="18">
-      <c r="C18" s="10"/>
+    <row r="18" spans="1:14" ht="18">
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -12156,10 +12206,13 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:13" ht="18">
-      <c r="C19" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" ht="18">
+      <c r="A19" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -12168,80 +12221,78 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:13" ht="18">
-      <c r="A20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" ht="18">
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="12"/>
-    </row>
-    <row r="21" spans="1:13" ht="18">
-      <c r="C21" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" ht="18">
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="I21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="12"/>
-    </row>
-    <row r="22" spans="1:13" ht="18">
-      <c r="C22" s="10"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" ht="18">
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:13" ht="18">
-      <c r="C23" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" ht="18">
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:13" ht="18">
-      <c r="C24" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:14" ht="18">
       <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="12"/>
-    </row>
-    <row r="25" spans="1:13" ht="18">
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" ht="18">
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" ht="18">
-      <c r="C26" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" ht="18">
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -12250,11 +12301,11 @@
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" ht="18">
-      <c r="C27" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" ht="18">
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -12263,11 +12314,11 @@
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" ht="18">
-      <c r="C28" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" ht="18">
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -12276,69 +12327,57 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" ht="18">
-      <c r="C29" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" ht="18">
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" ht="18">
-      <c r="C30" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" ht="18">
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="I30" s="10"/>
       <c r="K30" s="10"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" ht="18">
-      <c r="C31" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" ht="18">
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="I31" s="10"/>
       <c r="K31" s="10"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" ht="18">
-      <c r="C32" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" ht="18">
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="J32" s="10"/>
+      <c r="I32" s="10"/>
       <c r="K32" s="10"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="13"/>
-    </row>
-    <row r="33" spans="3:13" ht="18">
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="13"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>